<commit_message>
sanırım inventory sorunu çözüldü
</commit_message>
<xml_diff>
--- a/sellerflash-otomasyon-linkler/Food Service Equipment & Supplies.xlsx
+++ b/sellerflash-otomasyon-linkler/Food Service Equipment & Supplies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nihat/Documents/sellerflash-otomasyon-linkler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nihat/Documents/AmazonIcinGelistirdiklerim/amazon-seller-flash-otomasyonu-url/sellerflash-otomasyon-linkler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B1634E-A441-C446-BEB8-0EB47B5EFACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F9AF69-004E-6E40-8A70-B4F1593284CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="740" windowWidth="25900" windowHeight="17020" xr2:uid="{3990C341-BE15-C249-9C35-465A15D2EFB3}"/>
+    <workbookView xWindow="3500" yWindow="740" windowWidth="25900" windowHeight="16900" xr2:uid="{3990C341-BE15-C249-9C35-465A15D2EFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB283BC-FD09-FC4B-BC08-490F1BF99E76}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>